<commit_message>
BoM / board update
</commit_message>
<xml_diff>
--- a/BOM esp v2.xlsx
+++ b/BOM esp v2.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
-  <si>
-    <t>lm1117 3.3V SMD package</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Micro USB connector SMD two shield legs</t>
   </si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>arduino pro mini 3.3V 8MHz</t>
+  </si>
+  <si>
+    <t>lm1117 3.3V SOT-223 SMD package</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -449,13 +449,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -463,10 +463,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -474,10 +474,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -485,10 +485,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -496,10 +496,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -507,10 +507,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -518,10 +518,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -529,10 +529,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -540,10 +540,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -551,10 +551,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -562,15 +562,18 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -578,10 +581,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
         <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -589,10 +592,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -600,10 +603,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -611,10 +614,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -622,10 +625,10 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -633,10 +636,10 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -644,10 +647,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>